<commit_message>
bom. jlc pcb part confirmed
</commit_message>
<xml_diff>
--- a/slime_tracker_bom.xlsx
+++ b/slime_tracker_bom.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="144">
   <si>
     <t>Reference</t>
   </si>
@@ -151,14 +151,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Capacitor_Tantalum_SMD:CP_EIA-6032-15_Kemet-U</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>C123720</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>C9,C10</t>
   </si>
   <si>
@@ -279,9 +271,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>175mΩ 2.4A 2.5A 6.8uH Molded Inductor ±20% SMD,4.4x4.2mm Power Inductors ROHS</t>
-  </si>
-  <si>
     <t>slime:FXL0420</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -522,6 +511,14 @@
   </si>
   <si>
     <t>C206167</t>
+  </si>
+  <si>
+    <t>Capacitor_Tantalum_SMD:CASE-B-3528-21(mm) kemet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C600583</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -894,8 +891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1091,10 +1088,10 @@
         <v>35</v>
       </c>
       <c r="G9" t="s">
-        <v>36</v>
+        <v>142</v>
       </c>
       <c r="H9" t="s">
-        <v>37</v>
+        <v>143</v>
       </c>
       <c r="I9" t="s">
         <v>13</v>
@@ -1102,19 +1099,19 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B10">
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G10" t="s">
         <v>16</v>
       </c>
       <c r="H10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I10" t="s">
         <v>13</v>
@@ -1122,7 +1119,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -1134,7 +1131,7 @@
         <v>16</v>
       </c>
       <c r="H11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I11" t="s">
         <v>13</v>
@@ -1142,19 +1139,19 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" t="s">
         <v>43</v>
       </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="H12" t="s">
         <v>44</v>
-      </c>
-      <c r="G12" t="s">
-        <v>45</v>
-      </c>
-      <c r="H12" t="s">
-        <v>46</v>
       </c>
       <c r="I12" t="s">
         <v>13</v>
@@ -1162,19 +1159,19 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>46</v>
+      </c>
+      <c r="G13" t="s">
+        <v>43</v>
+      </c>
+      <c r="H13" t="s">
         <v>47</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
-        <v>48</v>
-      </c>
-      <c r="G13" t="s">
-        <v>45</v>
-      </c>
-      <c r="H13" t="s">
-        <v>49</v>
       </c>
       <c r="I13" t="s">
         <v>13</v>
@@ -1182,19 +1179,19 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
+        <v>49</v>
+      </c>
+      <c r="G14" t="s">
+        <v>50</v>
+      </c>
+      <c r="H14" t="s">
         <v>51</v>
-      </c>
-      <c r="G14" t="s">
-        <v>52</v>
-      </c>
-      <c r="H14" t="s">
-        <v>53</v>
       </c>
       <c r="I14" t="s">
         <v>13</v>
@@ -1202,94 +1199,92 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" t="s">
         <v>55</v>
       </c>
-      <c r="D15" t="s">
+      <c r="F15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" t="s">
         <v>56</v>
       </c>
-      <c r="E15" t="s">
+      <c r="H15" t="s">
         <v>57</v>
-      </c>
-      <c r="F15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G15" t="s">
-        <v>58</v>
-      </c>
-      <c r="H15" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" t="s">
         <v>60</v>
       </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="E16" t="s">
         <v>61</v>
       </c>
-      <c r="D16" t="s">
+      <c r="F16" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" t="s">
+        <v>57</v>
+      </c>
+      <c r="H16" t="s">
         <v>62</v>
-      </c>
-      <c r="E16" t="s">
-        <v>63</v>
-      </c>
-      <c r="F16" t="s">
-        <v>13</v>
-      </c>
-      <c r="G16" t="s">
-        <v>59</v>
-      </c>
-      <c r="H16" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>64</v>
+      </c>
+      <c r="G17" t="s">
         <v>65</v>
       </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="H17" t="s">
         <v>66</v>
       </c>
-      <c r="G17" t="s">
+      <c r="I17" s="3" t="s">
         <v>67</v>
-      </c>
-      <c r="H17" t="s">
-        <v>68</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>69</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="G18" t="s">
         <v>70</v>
       </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="H18" t="s">
         <v>71</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="G18" t="s">
-        <v>73</v>
-      </c>
-      <c r="H18" t="s">
-        <v>74</v>
       </c>
       <c r="I18" t="s">
         <v>13</v>
@@ -1297,19 +1292,19 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G19" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H19" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I19" t="s">
         <v>13</v>
@@ -1317,19 +1312,19 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B20">
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G20" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H20" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="I20" t="s">
         <v>13</v>
@@ -1337,19 +1332,19 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B21">
         <v>4</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G21" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H21" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="I21" t="s">
         <v>13</v>
@@ -1357,19 +1352,19 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G22" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H22" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="I22" t="s">
         <v>13</v>
@@ -1377,19 +1372,19 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G23" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H23" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="I23" t="s">
         <v>13</v>
@@ -1397,19 +1392,19 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G24" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H24" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="I24" t="s">
         <v>13</v>
@@ -1417,19 +1412,19 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B25">
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G25" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H25" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="I25" t="s">
         <v>13</v>
@@ -1437,19 +1432,19 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G26" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H26" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="I26" t="s">
         <v>13</v>
@@ -1457,19 +1452,19 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G27" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H27" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I27" t="s">
         <v>13</v>
@@ -1477,19 +1472,19 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B28">
         <v>2</v>
       </c>
       <c r="C28" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G28" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H28" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="I28" t="s">
         <v>13</v>
@@ -1497,19 +1492,19 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
+        <v>103</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>104</v>
+      </c>
+      <c r="G29" t="s">
+        <v>105</v>
+      </c>
+      <c r="H29" t="s">
         <v>106</v>
-      </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-      <c r="C29" t="s">
-        <v>107</v>
-      </c>
-      <c r="G29" t="s">
-        <v>108</v>
-      </c>
-      <c r="H29" t="s">
-        <v>109</v>
       </c>
       <c r="I29" t="s">
         <v>13</v>
@@ -1517,19 +1512,19 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B30">
         <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="G30" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H30" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="I30" t="s">
         <v>13</v>
@@ -1537,45 +1532,45 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D31" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E31" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F31" t="s">
         <v>13</v>
       </c>
       <c r="G31" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H31" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="G32" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="H32" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I32" t="s">
         <v>13</v>
@@ -1583,19 +1578,19 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="G33" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="H33" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I33" t="s">
         <v>13</v>
@@ -1603,19 +1598,19 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G34" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="H34" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I34" t="s">
         <v>13</v>
@@ -1623,19 +1618,19 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="G35" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="H35" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I35" t="s">
         <v>13</v>
@@ -1643,19 +1638,19 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="G36" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="H36" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I36" t="s">
         <v>13</v>
@@ -1663,24 +1658,24 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
+        <v>124</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37" t="s">
+        <v>125</v>
+      </c>
+      <c r="G37" t="s">
+        <v>126</v>
+      </c>
+      <c r="H37" t="s">
         <v>127</v>
-      </c>
-      <c r="B37">
-        <v>1</v>
-      </c>
-      <c r="C37" t="s">
-        <v>128</v>
-      </c>
-      <c r="G37" t="s">
-        <v>129</v>
-      </c>
-      <c r="H37" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -1689,79 +1684,79 @@
         <v>13</v>
       </c>
       <c r="D38" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E38" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F38" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G38" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H38" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
+        <v>131</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39" t="s">
+        <v>132</v>
+      </c>
+      <c r="G39" t="s">
+        <v>133</v>
+      </c>
+      <c r="H39" t="s">
         <v>134</v>
-      </c>
-      <c r="B39">
-        <v>1</v>
-      </c>
-      <c r="C39" t="s">
-        <v>135</v>
-      </c>
-      <c r="G39" t="s">
-        <v>136</v>
-      </c>
-      <c r="H39" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B40">
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D40" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E40" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F40" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G40" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H40" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
+        <v>138</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41" t="s">
+        <v>139</v>
+      </c>
+      <c r="G41" t="s">
+        <v>140</v>
+      </c>
+      <c r="H41" t="s">
         <v>141</v>
-      </c>
-      <c r="B41">
-        <v>1</v>
-      </c>
-      <c r="C41" t="s">
-        <v>142</v>
-      </c>
-      <c r="G41" t="s">
-        <v>143</v>
-      </c>
-      <c r="H41" t="s">
-        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>